<commit_message>
feat: Add IAQ parameter plots
</commit_message>
<xml_diff>
--- a/Data/room_info.xlsx
+++ b/Data/room_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD96F3B-EFF6-4AFB-9510-FC85A2FC87DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EF2AD3-A7C2-4CD1-9B4F-1BB002088419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>K1N0624</t>
   </si>
   <si>
-    <t>N/NE</t>
-  </si>
-  <si>
     <t>K3N0618</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Room_ID</t>
   </si>
   <si>
-    <t>Persons</t>
-  </si>
-  <si>
     <t>K3N0605</t>
   </si>
   <si>
@@ -82,15 +76,6 @@
     <t>Date (App)</t>
   </si>
   <si>
-    <t>App users</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>Room Type</t>
   </si>
   <si>
@@ -101,6 +86,21 @@
   </si>
   <si>
     <t>Area [m2]</t>
+  </si>
+  <si>
+    <t>No of Persons</t>
+  </si>
+  <si>
+    <t>No of App Users</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>North East</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,39 +439,39 @@
     <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -482,13 +482,13 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>1</v>
@@ -506,19 +506,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>1</v>
@@ -538,19 +538,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -562,23 +562,25 @@
         <v>43497</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>1</v>
@@ -604,13 +606,13 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -630,19 +632,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="b">
         <v>1</v>
@@ -662,19 +664,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="b">
         <v>1</v>
@@ -694,19 +696,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="b">
         <v>1</v>
@@ -718,23 +720,25 @@
         <v>43720</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="b">
         <v>0</v>
@@ -744,23 +748,25 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="b">
         <v>0</v>
@@ -770,23 +776,25 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="b">
         <v>0</v>
@@ -796,23 +804,25 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="b">
         <v>0</v>
@@ -822,7 +832,9 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:K13">

</xml_diff>